<commit_message>
LoginData.xlsx and properties files are modified
</commit_message>
<xml_diff>
--- a/src/main/java/com/inetbanking/testData/LoginData.xlsx
+++ b/src/main/java/com/inetbanking/testData/LoginData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>azezUqY</t>
+  </si>
+  <si>
+    <t>mngr212597</t>
+  </si>
+  <si>
+    <t>urEguzu</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,10 +449,10 @@
     </row>
     <row r="2" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
@@ -459,10 +465,10 @@
     </row>
     <row r="4" spans="1:2" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.3"/>

</xml_diff>